<commit_message>
sök funktion verkar funka
</commit_message>
<xml_diff>
--- a/fris.xlsx
+++ b/fris.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jens.lundeqvist\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jens.lundeqvist\programmering\webbutv\xceltest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E06D3A3-16ED-4F3A-9607-B4B41AA2F579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39340193-8457-447E-A748-054AD8682A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>produkt</t>
   </si>
@@ -48,12 +48,24 @@
   </si>
   <si>
     <t>pris</t>
+  </si>
+  <si>
+    <t>maskin</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>fil</t>
+  </si>
+  <si>
+    <t>hätta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,6 +443,38 @@
         <v>3333</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>